<commit_message>
Dokumente erstellt und hinzugefügt
</commit_message>
<xml_diff>
--- a/swe-iot/docs/it002/SprintPlan.xlsx
+++ b/swe-iot/docs/it002/SprintPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>E1S1 Implementieren Sie die Funktion zum Abspielen eines Tones in der InternetButtonApiImpl. Schreiben Sie auch eine kleine Applikation die zeigt, dass die Melodie auch wirklich ertšnt (PlayDemoApp).</t>
   </si>
@@ -65,10 +65,13 @@
     <t>Status</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Sprint 2 behandelt aus Sprint 1 die noch offenen Aufgaben (2,3 &amp; 4)</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Beheben der Probleme von unterschiedlichen Dateiversionen</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -172,6 +175,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -531,134 +547,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="110.25" x14ac:dyDescent="0.5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <v>3</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3">
+        <v>7</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="110.25" x14ac:dyDescent="0.5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5">
-        <v>3</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5">
-        <v>3</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>